<commit_message>
Refractored some code. Added some function that were missing.
Started to implement importing excel from cad to create fc appoggi.
</commit_message>
<xml_diff>
--- a/TiaAddin-Spin-ExcelReader/Templates/TemplateAllarmiUtenze_Motori.xlsx
+++ b/TiaAddin-Spin-ExcelReader/Templates/TemplateAllarmiUtenze_Motori.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PARONETTO G\Documents\GitHub\TiaAddIn-Spin\TiaAddin-Spin-ExcelReader\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C7D47A-EA48-421E-B7F6-FC798A811392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F49D09D-E40B-4DFD-A899-27245047CB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27750" windowHeight="16440" xr2:uid="{22A793F4-95FD-4AFA-8F43-DC77A5638B57}"/>
   </bookViews>
@@ -360,9 +360,6 @@
     <t>VENT12</t>
   </si>
   <si>
-    <t>PerTipoAllarme</t>
-  </si>
-  <si>
     <t>Salta num. ogni fine gruppo</t>
   </si>
   <si>
@@ -397,6 +394,9 @@
   </si>
   <si>
     <t>Alm{num_allarme} - {nome_utenza}: Sovvratemperatura</t>
+  </si>
+  <si>
+    <t>PerUtenza</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -463,6 +463,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -780,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667AB657-9EF0-4E7D-B211-0DE4E07AFF8D}">
   <dimension ref="B2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +864,7 @@
         <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L4" t="s">
         <v>30</v>
@@ -871,7 +874,7 @@
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>195</v>
       </c>
       <c r="E5" t="s">
@@ -890,7 +893,7 @@
         <v>25</v>
       </c>
       <c r="K5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L5" t="s">
         <v>31</v>
@@ -913,7 +916,7 @@
         <v>25</v>
       </c>
       <c r="K6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L6" t="s">
         <v>31</v>
@@ -923,7 +926,7 @@
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>200</v>
       </c>
       <c r="E7" t="s">
@@ -942,7 +945,7 @@
         <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L7" t="s">
         <v>31</v>
@@ -971,7 +974,7 @@
         <v>25</v>
       </c>
       <c r="K8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L8" t="s">
         <v>31</v>
@@ -979,10 +982,10 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" t="s">
         <v>114</v>
-      </c>
-      <c r="C9" t="s">
-        <v>115</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -1000,7 +1003,7 @@
         <v>25</v>
       </c>
       <c r="K9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L9" t="s">
         <v>30</v>
@@ -1008,10 +1011,10 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
         <v>34</v>
@@ -1029,7 +1032,7 @@
         <v>25</v>
       </c>
       <c r="K10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L10" t="s">
         <v>31</v>
@@ -1037,10 +1040,10 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
+        <v>111</v>
+      </c>
+      <c r="C11" s="4">
+        <v>18</v>
       </c>
       <c r="E11" t="s">
         <v>35</v>
@@ -1058,7 +1061,7 @@
         <v>25</v>
       </c>
       <c r="K11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L11" t="s">
         <v>31</v>
@@ -1671,16 +1674,12 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:K2"/>
   </mergeCells>
-  <dataValidations count="6">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{F5E4D3FC-4D67-4AB1-A3E0-2BD5870384F2}">
       <formula1>"UnoPerSegmento,GruppoPerSegmento"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{F717952B-D4F9-4570-84C1-F92597681F3D}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7 C5" xr:uid="{F717952B-D4F9-4570-84C1-F92597681F3D}">
       <formula1>0</formula1>
-      <formula2>99999</formula2>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{CF56118D-FBE9-4E70-A77B-46B77A36FDC7}">
-      <formula1>1</formula1>
       <formula2>99999</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L11" xr:uid="{2F86C16C-0261-4A0E-9E02-68DD4F8930D4}">

</xml_diff>